<commit_message>
big update after enterprise setup
</commit_message>
<xml_diff>
--- a/sql query/Book1.xlsx
+++ b/sql query/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\upg automation\sql query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7705B620-9423-4AD3-BB01-AF4CD6F514F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD9D2C9-4CF5-4545-92FB-1B3FAFEAC3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R56"/>
+      <selection activeCell="F7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sql for approval category
</commit_message>
<xml_diff>
--- a/sql query/Book1.xlsx
+++ b/sql query/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\upg automation\sql query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD9D2C9-4CF5-4545-92FB-1B3FAFEAC3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5626678-727D-4221-9E5D-01F089B68F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="A1:XFD1048576"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>